<commit_message>
Test - ok: Tarefa01 e Participação Especial
</commit_message>
<xml_diff>
--- a/config/dados_trabalho.xlsx
+++ b/config/dados_trabalho.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DVOS\Documents\Github\Trabalho_AEPP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DVOS\Documents\Github\Trabalho_AEPP\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49F35D6F-D2C8-40A0-9D20-25436DCE0C2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81207445-FEA3-41AE-ADDB-6E022E8768A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Perfuracao" sheetId="7" r:id="rId1"/>
@@ -160,7 +160,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -185,6 +185,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -467,8 +468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBCA8598-302F-4D5C-896E-FDBCEF4EBD8E}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -523,10 +524,10 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="2">
+      <c r="A5" s="12">
         <v>1000</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="12">
         <v>6</v>
       </c>
       <c r="C5">
@@ -1017,8 +1018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection sqref="A1:C30"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1557,8 +1558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43F5FF6F-3640-47DB-A887-5158560668C6}">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection sqref="A1:C31"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1920,7 +1921,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{564D95AC-1F42-454D-8611-E2410C47CEBE}">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C31" sqref="B31:C31"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fix: Tarefa_02_Down - ok
</commit_message>
<xml_diff>
--- a/config/dados_trabalho.xlsx
+++ b/config/dados_trabalho.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DVOS\Documents\Github\Trabalho_AEPP\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81207445-FEA3-41AE-ADDB-6E022E8768A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9108DF66-3FB1-4B50-986F-331FB0A39959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Perfuracao" sheetId="7" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="7">
   <si>
     <t>Base</t>
   </si>
@@ -58,12 +58,6 @@
   </si>
   <si>
     <t>Ano</t>
-  </si>
-  <si>
-    <t>Pessimista</t>
-  </si>
-  <si>
-    <t>Otimista</t>
   </si>
   <si>
     <t>preco_broca</t>
@@ -185,7 +179,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -468,7 +464,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBCA8598-302F-4D5C-896E-FDBCEF4EBD8E}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -487,7 +483,7 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -524,10 +520,10 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="12">
+      <c r="A5">
         <v>1000</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5">
         <v>6</v>
       </c>
       <c r="C5">
@@ -553,8 +549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DCEB578-46D6-4B9C-8170-AAC088C30D0E}">
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -570,10 +566,10 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G1" s="6"/>
       <c r="J1" s="6"/>
@@ -585,7 +581,7 @@
       <c r="B2" s="1">
         <v>70</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="12">
         <v>70</v>
       </c>
       <c r="D2" s="1">
@@ -1018,7 +1014,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>

</xml_diff>